<commit_message>
version 1.0.3 - fixed some issues with reading files with incomplete lines
</commit_message>
<xml_diff>
--- a/testData/testStaticFieldBean.xlsx
+++ b/testData/testStaticFieldBean.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\LightweightFileObjectIO\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\LightweightBeanIO\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB2593D-6E44-488B-A8FA-752DF9DBE16F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51951336-5A79-44CC-9861-A3BEF388D6D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5658" yWindow="2004" windowWidth="14802" windowHeight="6630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1098" yWindow="1098" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>

</xml_diff>